<commit_message>
Setup replay memory, reinforce algorithm
</commit_message>
<xml_diff>
--- a/01_Projectmanagement/Time-tracking Vinz.xlsx
+++ b/01_Projectmanagement/Time-tracking Vinz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unibe365-my.sharepoint.com/personal/vinzenz_uhr_students_unibe_ch/Documents/Arbeit BFH/github/01_Projectmanagement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="11_AD4DB114E441178AC67DF43CCE52CDE2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE321A0A-34AD-40DE-877C-80F673F1D33F}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="11_AD4DB114E441178AC67DF43CCE52CDE2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18D53254-81E9-44B4-A657-C8E73C4C1AA8}"/>
   <bookViews>
-    <workbookView xWindow="29970" yWindow="1170" windowWidth="18900" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Time-tracking Vinz</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Research RL library Gymnasium, code RL env</t>
+  </si>
+  <si>
+    <t>27.08.</t>
+  </si>
+  <si>
+    <t>Code REINFORCE algo, replay memory, setup Ubelix</t>
   </si>
 </sst>
 </file>
@@ -437,22 +443,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -463,7 +469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -474,7 +480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -485,7 +491,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -496,7 +502,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -507,7 +513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -518,7 +524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -529,7 +535,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -540,19 +546,30 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>555</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="2" t="str">
         <f>_xlfn.CONCAT(SUM(B4:B15)," min")</f>
-        <v>2225 min</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+        <v>2780 min</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="str">
         <f>_xlfn.CONCAT("~",ROUND(SUM(B4:B15) / 60, 2)," h")</f>
-        <v>~37.08 h</v>
+        <v>~46.33 h</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjust reward, split notebook into modules, add comments
</commit_message>
<xml_diff>
--- a/01_Projectmanagement/Time-tracking Vinz.xlsx
+++ b/01_Projectmanagement/Time-tracking Vinz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unibe365-my.sharepoint.com/personal/vinzenz_uhr_students_unibe_ch/Documents/Arbeit BFH/github/01_Projectmanagement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="11_AD4DB114E441178AC67DF43CCE52CDE2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18D53254-81E9-44B4-A657-C8E73C4C1AA8}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="11_AD4DB114E441178AC67DF43CCE52CDE2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8C58C25-62A0-4A3A-84C6-1658A46CB5CB}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Time-tracking Vinz</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Code REINFORCE algo, replay memory, setup Ubelix</t>
+  </si>
+  <si>
+    <t>Setup ubelix, adjust reward, split in modules, add comments</t>
+  </si>
+  <si>
+    <t>28.08.</t>
   </si>
 </sst>
 </file>
@@ -444,21 +450,21 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -469,7 +475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -480,7 +486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -491,7 +497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -502,7 +508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -513,7 +519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -524,7 +530,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -535,7 +541,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -546,7 +552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -557,19 +563,30 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>460</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="2" t="str">
         <f>_xlfn.CONCAT(SUM(B4:B15)," min")</f>
-        <v>2780 min</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+        <v>3240 min</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="str">
         <f>_xlfn.CONCAT("~",ROUND(SUM(B4:B15) / 60, 2)," h")</f>
-        <v>~46.33 h</v>
+        <v>~54 h</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Introduce num_message_passing, merge two GNN to one
</commit_message>
<xml_diff>
--- a/01_Projectmanagement/Time-tracking Vinz.xlsx
+++ b/01_Projectmanagement/Time-tracking Vinz.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unibe365-my.sharepoint.com/personal/vinzenz_uhr_students_unibe_ch/Documents/Arbeit BFH/github/01_Projectmanagement/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinze\OneDrive - Universitaet Bern\Arbeit BFH\github\01_Projectmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="11_AD4DB114E441178AC67DF43CCE52CDE2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E346D5B-80DF-4857-809A-B1A37B9BEA7D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69989344-0E32-46A8-AC75-4F180A2F45A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Time-tracking Vinz</t>
   </si>
@@ -92,12 +92,6 @@
     <t>27.08.</t>
   </si>
   <si>
-    <t>Code REINFORCE algo, replay memory, setup Ubelix</t>
-  </si>
-  <si>
-    <t>Setup ubelix, adjust reward, split in modules, add comments</t>
-  </si>
-  <si>
     <t>28.08.</t>
   </si>
   <si>
@@ -105,6 +99,18 @@
   </si>
   <si>
     <t>Meeting + Preparation</t>
+  </si>
+  <si>
+    <t>30.08.</t>
+  </si>
+  <si>
+    <t>Setup ubelix, Code: adjust reward, split in modules, add comments</t>
+  </si>
+  <si>
+    <t>Setup Ubelix, Code: REINFORCE algo, replay memory</t>
+  </si>
+  <si>
+    <t>Code: Introduce num_message_passing, merge two gnn</t>
   </si>
 </sst>
 </file>
@@ -456,21 +462,21 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -481,7 +487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -492,7 +498,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -503,7 +509,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -514,7 +520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -525,7 +531,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -536,7 +542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -547,7 +553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -558,7 +564,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -566,44 +572,55 @@
         <v>555</v>
       </c>
       <c r="C11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>20</v>
       </c>
       <c r="B12">
         <v>460</v>
       </c>
       <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
       </c>
       <c r="B13">
         <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>95</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="2" t="str">
         <f>_xlfn.CONCAT(SUM(B4:B15)," min")</f>
-        <v>3305 min</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+        <v>3400 min</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="str">
         <f>_xlfn.CONCAT("~",ROUND(SUM(B4:B15) / 60, 2)," h")</f>
-        <v>~55.08 h</v>
+        <v>~56.67 h</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
introduce new evaluation metrics, adjust lr and reward scale
</commit_message>
<xml_diff>
--- a/01_Projectmanagement/Time-tracking Vinz.xlsx
+++ b/01_Projectmanagement/Time-tracking Vinz.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinze\OneDrive - Universitaet Bern\Arbeit BFH\github\01_Projectmanagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unibe365-my.sharepoint.com/personal/vinzenz_uhr_students_unibe_ch/Documents/Arbeit BFH/github/01_Projectmanagement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69989344-0E32-46A8-AC75-4F180A2F45A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{69989344-0E32-46A8-AC75-4F180A2F45A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D109257E-E9C9-4680-9DAB-7994D7519A3C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Time-tracking Vinz</t>
   </si>
@@ -111,6 +111,18 @@
   </si>
   <si>
     <t>Code: Introduce num_message_passing, merge two gnn</t>
+  </si>
+  <si>
+    <t>Code: Extend evaluation metrics, adjust lr, adjust reward weighting, troubleshooting</t>
+  </si>
+  <si>
+    <t>Code: adjust reward</t>
+  </si>
+  <si>
+    <t>31.08.</t>
+  </si>
+  <si>
+    <t>02.09.</t>
   </si>
 </sst>
 </file>
@@ -459,24 +471,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -487,7 +499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -498,7 +510,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -509,7 +521,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -520,7 +532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -531,7 +543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -542,7 +554,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -553,7 +565,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -564,7 +576,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -575,7 +587,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -586,7 +598,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -597,7 +609,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -608,19 +620,41 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <v>520</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="2" t="str">
-        <f>_xlfn.CONCAT(SUM(B4:B15)," min")</f>
-        <v>3400 min</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="str">
-        <f>_xlfn.CONCAT("~",ROUND(SUM(B4:B15) / 60, 2)," h")</f>
-        <v>~56.67 h</v>
+        <f>_xlfn.CONCAT(SUM(B4:B16)," min")</f>
+        <v>3995 min</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="str">
+        <f>_xlfn.CONCAT("~",ROUND(SUM(B4:B16) / 60, 2)," h")</f>
+        <v>~66.58 h</v>
       </c>
     </row>
   </sheetData>

</xml_diff>